<commit_message>
updated oilprice history data
</commit_message>
<xml_diff>
--- a/cui/data/crude_oil_monthly_history.xlsx
+++ b/cui/data/crude_oil_monthly_history.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26505"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tstomoki/home/python/navigation_simulator/cui/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="12800" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +37,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="178" formatCode="yyyy/m/d;@"/>
+    <numFmt numFmtId="176" formatCode="yyyy/m/d;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -81,16 +86,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -416,18 +426,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B352"/>
+  <dimension ref="A1:B360"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A339" workbookViewId="0">
+      <selection activeCell="E358" sqref="E358"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="12.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="50">
+    <row r="1" spans="1:2" ht="52" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -435,7 +445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
         <v>31427</v>
       </c>
@@ -443,7 +453,7 @@
         <v>22.93</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>31458</v>
       </c>
@@ -451,7 +461,7 @@
         <v>15.46</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>31486</v>
       </c>
@@ -459,7 +469,7 @@
         <v>12.61</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>31517</v>
       </c>
@@ -467,7 +477,7 @@
         <v>12.84</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>31547</v>
       </c>
@@ -475,7 +485,7 @@
         <v>15.38</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>31578</v>
       </c>
@@ -483,7 +493,7 @@
         <v>13.43</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>31608</v>
       </c>
@@ -491,7 +501,7 @@
         <v>11.59</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
         <v>31639</v>
       </c>
@@ -499,7 +509,7 @@
         <v>15.1</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>31670</v>
       </c>
@@ -507,7 +517,7 @@
         <v>14.87</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
         <v>31700</v>
       </c>
@@ -515,7 +525,7 @@
         <v>14.9</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
         <v>31731</v>
       </c>
@@ -523,7 +533,7 @@
         <v>15.22</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
         <v>31761</v>
       </c>
@@ -531,7 +541,7 @@
         <v>16.11</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
         <v>31792</v>
       </c>
@@ -539,7 +549,7 @@
         <v>18.649999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
         <v>31823</v>
       </c>
@@ -547,7 +557,7 @@
         <v>17.75</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16" s="3">
         <v>31851</v>
       </c>
@@ -555,7 +565,7 @@
         <v>18.3</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" s="3">
         <v>31882</v>
       </c>
@@ -563,7 +573,7 @@
         <v>18.68</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" s="3">
         <v>31912</v>
       </c>
@@ -571,7 +581,7 @@
         <v>19.440000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" s="3">
         <v>31943</v>
       </c>
@@ -579,7 +589,7 @@
         <v>20.07</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" s="3">
         <v>31973</v>
       </c>
@@ -587,7 +597,7 @@
         <v>21.34</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" s="3">
         <v>32004</v>
       </c>
@@ -595,7 +605,7 @@
         <v>20.309999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" s="3">
         <v>32035</v>
       </c>
@@ -603,7 +613,7 @@
         <v>19.53</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23" s="3">
         <v>32065</v>
       </c>
@@ -611,7 +621,7 @@
         <v>19.86</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" s="3">
         <v>32096</v>
       </c>
@@ -619,7 +629,7 @@
         <v>18.850000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25" s="3">
         <v>32126</v>
       </c>
@@ -627,7 +637,7 @@
         <v>17.28</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A26" s="3">
         <v>32157</v>
       </c>
@@ -635,7 +645,7 @@
         <v>17.13</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" s="3">
         <v>32188</v>
       </c>
@@ -643,7 +653,7 @@
         <v>16.8</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A28" s="3">
         <v>32217</v>
       </c>
@@ -651,7 +661,7 @@
         <v>16.2</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A29" s="3">
         <v>32248</v>
       </c>
@@ -659,7 +669,7 @@
         <v>17.86</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A30" s="3">
         <v>32278</v>
       </c>
@@ -667,7 +677,7 @@
         <v>17.420000000000002</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A31" s="3">
         <v>32309</v>
       </c>
@@ -675,7 +685,7 @@
         <v>16.53</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A32" s="3">
         <v>32339</v>
       </c>
@@ -683,7 +693,7 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A33" s="3">
         <v>32370</v>
       </c>
@@ -691,7 +701,7 @@
         <v>15.52</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A34" s="3">
         <v>32401</v>
       </c>
@@ -699,7 +709,7 @@
         <v>14.54</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A35" s="3">
         <v>32431</v>
       </c>
@@ -707,7 +717,7 @@
         <v>13.77</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A36" s="3">
         <v>32462</v>
       </c>
@@ -715,7 +725,7 @@
         <v>14.14</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A37" s="3">
         <v>32492</v>
       </c>
@@ -723,7 +733,7 @@
         <v>16.38</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A38" s="3">
         <v>32523</v>
       </c>
@@ -731,7 +741,7 @@
         <v>18.02</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A39" s="3">
         <v>32554</v>
       </c>
@@ -739,7 +749,7 @@
         <v>17.940000000000001</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A40" s="3">
         <v>32582</v>
       </c>
@@ -747,7 +757,7 @@
         <v>19.48</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A41" s="3">
         <v>32613</v>
       </c>
@@ -755,7 +765,7 @@
         <v>21.07</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A42" s="3">
         <v>32643</v>
       </c>
@@ -763,7 +773,7 @@
         <v>20.12</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A43" s="3">
         <v>32674</v>
       </c>
@@ -771,7 +781,7 @@
         <v>20.05</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A44" s="3">
         <v>32704</v>
       </c>
@@ -779,7 +789,7 @@
         <v>19.78</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A45" s="3">
         <v>32735</v>
       </c>
@@ -787,7 +797,7 @@
         <v>18.579999999999998</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A46" s="3">
         <v>32766</v>
       </c>
@@ -795,7 +805,7 @@
         <v>19.59</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A47" s="3">
         <v>32796</v>
       </c>
@@ -803,7 +813,7 @@
         <v>20.100000000000001</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A48" s="3">
         <v>32827</v>
       </c>
@@ -811,7 +821,7 @@
         <v>19.86</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A49" s="3">
         <v>32857</v>
       </c>
@@ -819,7 +829,7 @@
         <v>21.1</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A50" s="3">
         <v>32888</v>
       </c>
@@ -827,7 +837,7 @@
         <v>22.86</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A51" s="3">
         <v>32919</v>
       </c>
@@ -835,7 +845,7 @@
         <v>22.11</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A52" s="3">
         <v>32947</v>
       </c>
@@ -843,7 +853,7 @@
         <v>20.39</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A53" s="3">
         <v>32978</v>
       </c>
@@ -851,7 +861,7 @@
         <v>18.43</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A54" s="3">
         <v>33008</v>
       </c>
@@ -859,7 +869,7 @@
         <v>18.2</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A55" s="3">
         <v>33039</v>
       </c>
@@ -867,7 +877,7 @@
         <v>16.7</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A56" s="3">
         <v>33069</v>
       </c>
@@ -875,7 +885,7 @@
         <v>18.45</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A57" s="3">
         <v>33100</v>
       </c>
@@ -883,7 +893,7 @@
         <v>27.31</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A58" s="3">
         <v>33131</v>
       </c>
@@ -891,7 +901,7 @@
         <v>33.51</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A59" s="3">
         <v>33161</v>
       </c>
@@ -899,7 +909,7 @@
         <v>36.04</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A60" s="3">
         <v>33192</v>
       </c>
@@ -907,7 +917,7 @@
         <v>32.33</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A61" s="3">
         <v>33222</v>
       </c>
@@ -915,7 +925,7 @@
         <v>27.28</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A62" s="3">
         <v>33253</v>
       </c>
@@ -923,7 +933,7 @@
         <v>25.23</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A63" s="3">
         <v>33284</v>
       </c>
@@ -931,7 +941,7 @@
         <v>20.48</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A64" s="3">
         <v>33312</v>
       </c>
@@ -939,7 +949,7 @@
         <v>19.899999999999999</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A65" s="3">
         <v>33343</v>
       </c>
@@ -947,7 +957,7 @@
         <v>20.83</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A66" s="3">
         <v>33373</v>
       </c>
@@ -955,7 +965,7 @@
         <v>21.23</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A67" s="3">
         <v>33404</v>
       </c>
@@ -963,7 +973,7 @@
         <v>20.190000000000001</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A68" s="3">
         <v>33434</v>
       </c>
@@ -971,7 +981,7 @@
         <v>21.4</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A69" s="3">
         <v>33465</v>
       </c>
@@ -979,7 +989,7 @@
         <v>21.69</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A70" s="3">
         <v>33496</v>
       </c>
@@ -987,7 +997,7 @@
         <v>21.89</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A71" s="3">
         <v>33526</v>
       </c>
@@ -995,7 +1005,7 @@
         <v>23.23</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A72" s="3">
         <v>33557</v>
       </c>
@@ -1003,7 +1013,7 @@
         <v>22.46</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A73" s="3">
         <v>33587</v>
       </c>
@@ -1011,7 +1021,7 @@
         <v>19.5</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A74" s="3">
         <v>33618</v>
       </c>
@@ -1019,7 +1029,7 @@
         <v>18.79</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A75" s="3">
         <v>33649</v>
       </c>
@@ -1027,7 +1037,7 @@
         <v>19.010000000000002</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A76" s="3">
         <v>33678</v>
       </c>
@@ -1035,7 +1045,7 @@
         <v>18.920000000000002</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A77" s="3">
         <v>33709</v>
       </c>
@@ -1043,7 +1053,7 @@
         <v>20.23</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A78" s="3">
         <v>33739</v>
       </c>
@@ -1051,7 +1061,7 @@
         <v>20.98</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A79" s="3">
         <v>33770</v>
       </c>
@@ -1059,7 +1069,7 @@
         <v>22.39</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A80" s="3">
         <v>33800</v>
       </c>
@@ -1067,7 +1077,7 @@
         <v>21.78</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A81" s="3">
         <v>33831</v>
       </c>
@@ -1075,7 +1085,7 @@
         <v>21.34</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A82" s="3">
         <v>33862</v>
       </c>
@@ -1083,7 +1093,7 @@
         <v>21.88</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A83" s="3">
         <v>33892</v>
       </c>
@@ -1091,7 +1101,7 @@
         <v>21.69</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A84" s="3">
         <v>33923</v>
       </c>
@@ -1099,7 +1109,7 @@
         <v>20.34</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A85" s="3">
         <v>33953</v>
       </c>
@@ -1107,7 +1117,7 @@
         <v>19.41</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A86" s="3">
         <v>33984</v>
       </c>
@@ -1115,7 +1125,7 @@
         <v>19.03</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A87" s="3">
         <v>34015</v>
       </c>
@@ -1123,7 +1133,7 @@
         <v>20.09</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A88" s="3">
         <v>34043</v>
       </c>
@@ -1131,7 +1141,7 @@
         <v>20.32</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A89" s="3">
         <v>34074</v>
       </c>
@@ -1139,7 +1149,7 @@
         <v>20.25</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A90" s="3">
         <v>34104</v>
       </c>
@@ -1147,7 +1157,7 @@
         <v>19.95</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A91" s="3">
         <v>34135</v>
       </c>
@@ -1155,7 +1165,7 @@
         <v>19.09</v>
       </c>
     </row>
-    <row r="92" spans="1:2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A92" s="3">
         <v>34165</v>
       </c>
@@ -1163,7 +1173,7 @@
         <v>17.89</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A93" s="3">
         <v>34196</v>
       </c>
@@ -1171,7 +1181,7 @@
         <v>18.010000000000002</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A94" s="3">
         <v>34227</v>
       </c>
@@ -1179,7 +1189,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A95" s="3">
         <v>34257</v>
       </c>
@@ -1187,7 +1197,7 @@
         <v>18.149999999999999</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A96" s="3">
         <v>34288</v>
       </c>
@@ -1195,7 +1205,7 @@
         <v>16.61</v>
       </c>
     </row>
-    <row r="97" spans="1:2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A97" s="3">
         <v>34318</v>
       </c>
@@ -1203,7 +1213,7 @@
         <v>14.52</v>
       </c>
     </row>
-    <row r="98" spans="1:2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A98" s="3">
         <v>34349</v>
       </c>
@@ -1211,7 +1221,7 @@
         <v>15.03</v>
       </c>
     </row>
-    <row r="99" spans="1:2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A99" s="3">
         <v>34380</v>
       </c>
@@ -1219,7 +1229,7 @@
         <v>14.78</v>
       </c>
     </row>
-    <row r="100" spans="1:2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A100" s="3">
         <v>34408</v>
       </c>
@@ -1227,7 +1237,7 @@
         <v>14.68</v>
       </c>
     </row>
-    <row r="101" spans="1:2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A101" s="3">
         <v>34439</v>
       </c>
@@ -1235,7 +1245,7 @@
         <v>16.420000000000002</v>
       </c>
     </row>
-    <row r="102" spans="1:2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A102" s="3">
         <v>34469</v>
       </c>
@@ -1243,7 +1253,7 @@
         <v>17.89</v>
       </c>
     </row>
-    <row r="103" spans="1:2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A103" s="3">
         <v>34500</v>
       </c>
@@ -1251,7 +1261,7 @@
         <v>19.059999999999999</v>
       </c>
     </row>
-    <row r="104" spans="1:2">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A104" s="3">
         <v>34530</v>
       </c>
@@ -1259,7 +1269,7 @@
         <v>19.66</v>
       </c>
     </row>
-    <row r="105" spans="1:2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A105" s="3">
         <v>34561</v>
       </c>
@@ -1267,7 +1277,7 @@
         <v>18.38</v>
       </c>
     </row>
-    <row r="106" spans="1:2">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A106" s="3">
         <v>34592</v>
       </c>
@@ -1275,7 +1285,7 @@
         <v>17.45</v>
       </c>
     </row>
-    <row r="107" spans="1:2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A107" s="3">
         <v>34622</v>
       </c>
@@ -1283,7 +1293,7 @@
         <v>17.72</v>
       </c>
     </row>
-    <row r="108" spans="1:2">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A108" s="3">
         <v>34653</v>
       </c>
@@ -1291,7 +1301,7 @@
         <v>18.07</v>
       </c>
     </row>
-    <row r="109" spans="1:2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A109" s="3">
         <v>34683</v>
       </c>
@@ -1299,7 +1309,7 @@
         <v>17.16</v>
       </c>
     </row>
-    <row r="110" spans="1:2">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A110" s="3">
         <v>34714</v>
       </c>
@@ -1307,7 +1317,7 @@
         <v>18.04</v>
       </c>
     </row>
-    <row r="111" spans="1:2">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A111" s="3">
         <v>34745</v>
       </c>
@@ -1315,7 +1325,7 @@
         <v>18.57</v>
       </c>
     </row>
-    <row r="112" spans="1:2">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A112" s="3">
         <v>34773</v>
       </c>
@@ -1323,7 +1333,7 @@
         <v>18.54</v>
       </c>
     </row>
-    <row r="113" spans="1:2">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A113" s="3">
         <v>34804</v>
       </c>
@@ -1331,7 +1341,7 @@
         <v>19.899999999999999</v>
       </c>
     </row>
-    <row r="114" spans="1:2">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A114" s="3">
         <v>34834</v>
       </c>
@@ -1339,7 +1349,7 @@
         <v>19.739999999999998</v>
       </c>
     </row>
-    <row r="115" spans="1:2">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A115" s="3">
         <v>34865</v>
       </c>
@@ -1347,7 +1357,7 @@
         <v>18.45</v>
       </c>
     </row>
-    <row r="116" spans="1:2">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A116" s="3">
         <v>34895</v>
       </c>
@@ -1355,7 +1365,7 @@
         <v>17.329999999999998</v>
       </c>
     </row>
-    <row r="117" spans="1:2">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A117" s="3">
         <v>34926</v>
       </c>
@@ -1363,7 +1373,7 @@
         <v>18.02</v>
       </c>
     </row>
-    <row r="118" spans="1:2">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A118" s="3">
         <v>34957</v>
       </c>
@@ -1371,7 +1381,7 @@
         <v>18.23</v>
       </c>
     </row>
-    <row r="119" spans="1:2">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A119" s="3">
         <v>34987</v>
       </c>
@@ -1379,7 +1389,7 @@
         <v>17.43</v>
       </c>
     </row>
-    <row r="120" spans="1:2">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A120" s="3">
         <v>35018</v>
       </c>
@@ -1387,7 +1397,7 @@
         <v>17.989999999999998</v>
       </c>
     </row>
-    <row r="121" spans="1:2">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A121" s="3">
         <v>35048</v>
       </c>
@@ -1395,7 +1405,7 @@
         <v>19.03</v>
       </c>
     </row>
-    <row r="122" spans="1:2">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A122" s="3">
         <v>35079</v>
       </c>
@@ -1403,7 +1413,7 @@
         <v>18.86</v>
       </c>
     </row>
-    <row r="123" spans="1:2">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A123" s="3">
         <v>35110</v>
       </c>
@@ -1411,7 +1421,7 @@
         <v>19.09</v>
       </c>
     </row>
-    <row r="124" spans="1:2">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A124" s="3">
         <v>35139</v>
       </c>
@@ -1419,7 +1429,7 @@
         <v>21.33</v>
       </c>
     </row>
-    <row r="125" spans="1:2">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A125" s="3">
         <v>35170</v>
       </c>
@@ -1427,7 +1437,7 @@
         <v>23.5</v>
       </c>
     </row>
-    <row r="126" spans="1:2">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A126" s="3">
         <v>35200</v>
       </c>
@@ -1435,7 +1445,7 @@
         <v>21.17</v>
       </c>
     </row>
-    <row r="127" spans="1:2">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A127" s="3">
         <v>35231</v>
       </c>
@@ -1443,7 +1453,7 @@
         <v>20.420000000000002</v>
       </c>
     </row>
-    <row r="128" spans="1:2">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A128" s="3">
         <v>35261</v>
       </c>
@@ -1451,7 +1461,7 @@
         <v>21.3</v>
       </c>
     </row>
-    <row r="129" spans="1:2">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A129" s="3">
         <v>35292</v>
       </c>
@@ -1459,7 +1469,7 @@
         <v>21.9</v>
       </c>
     </row>
-    <row r="130" spans="1:2">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A130" s="3">
         <v>35323</v>
       </c>
@@ -1467,7 +1477,7 @@
         <v>23.97</v>
       </c>
     </row>
-    <row r="131" spans="1:2">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A131" s="3">
         <v>35353</v>
       </c>
@@ -1475,7 +1485,7 @@
         <v>24.88</v>
       </c>
     </row>
-    <row r="132" spans="1:2">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A132" s="3">
         <v>35384</v>
       </c>
@@ -1483,7 +1493,7 @@
         <v>23.71</v>
       </c>
     </row>
-    <row r="133" spans="1:2">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A133" s="3">
         <v>35414</v>
       </c>
@@ -1491,7 +1501,7 @@
         <v>25.23</v>
       </c>
     </row>
-    <row r="134" spans="1:2">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A134" s="3">
         <v>35445</v>
       </c>
@@ -1499,7 +1509,7 @@
         <v>25.13</v>
       </c>
     </row>
-    <row r="135" spans="1:2">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A135" s="3">
         <v>35476</v>
       </c>
@@ -1507,7 +1517,7 @@
         <v>22.18</v>
       </c>
     </row>
-    <row r="136" spans="1:2">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A136" s="3">
         <v>35504</v>
       </c>
@@ -1515,7 +1525,7 @@
         <v>20.97</v>
       </c>
     </row>
-    <row r="137" spans="1:2">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A137" s="3">
         <v>35535</v>
       </c>
@@ -1523,7 +1533,7 @@
         <v>19.7</v>
       </c>
     </row>
-    <row r="138" spans="1:2">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A138" s="3">
         <v>35565</v>
       </c>
@@ -1531,7 +1541,7 @@
         <v>20.82</v>
       </c>
     </row>
-    <row r="139" spans="1:2">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A139" s="3">
         <v>35596</v>
       </c>
@@ -1539,7 +1549,7 @@
         <v>19.260000000000002</v>
       </c>
     </row>
-    <row r="140" spans="1:2">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A140" s="3">
         <v>35626</v>
       </c>
@@ -1547,7 +1557,7 @@
         <v>19.66</v>
       </c>
     </row>
-    <row r="141" spans="1:2">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A141" s="3">
         <v>35657</v>
       </c>
@@ -1555,7 +1565,7 @@
         <v>19.95</v>
       </c>
     </row>
-    <row r="142" spans="1:2">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A142" s="3">
         <v>35688</v>
       </c>
@@ -1563,7 +1573,7 @@
         <v>19.8</v>
       </c>
     </row>
-    <row r="143" spans="1:2">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A143" s="3">
         <v>35718</v>
       </c>
@@ -1571,7 +1581,7 @@
         <v>21.33</v>
       </c>
     </row>
-    <row r="144" spans="1:2">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A144" s="3">
         <v>35749</v>
       </c>
@@ -1579,7 +1589,7 @@
         <v>20.190000000000001</v>
       </c>
     </row>
-    <row r="145" spans="1:2">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A145" s="3">
         <v>35779</v>
       </c>
@@ -1587,7 +1597,7 @@
         <v>18.329999999999998</v>
       </c>
     </row>
-    <row r="146" spans="1:2">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A146" s="3">
         <v>35810</v>
       </c>
@@ -1595,7 +1605,7 @@
         <v>16.72</v>
       </c>
     </row>
-    <row r="147" spans="1:2">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A147" s="3">
         <v>35841</v>
       </c>
@@ -1603,7 +1613,7 @@
         <v>16.059999999999999</v>
       </c>
     </row>
-    <row r="148" spans="1:2">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A148" s="3">
         <v>35869</v>
       </c>
@@ -1611,7 +1621,7 @@
         <v>15.12</v>
       </c>
     </row>
-    <row r="149" spans="1:2">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A149" s="3">
         <v>35900</v>
       </c>
@@ -1619,7 +1629,7 @@
         <v>15.35</v>
       </c>
     </row>
-    <row r="150" spans="1:2">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A150" s="3">
         <v>35930</v>
       </c>
@@ -1627,7 +1637,7 @@
         <v>14.91</v>
       </c>
     </row>
-    <row r="151" spans="1:2">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A151" s="3">
         <v>35961</v>
       </c>
@@ -1635,7 +1645,7 @@
         <v>13.72</v>
       </c>
     </row>
-    <row r="152" spans="1:2">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A152" s="3">
         <v>35991</v>
       </c>
@@ -1643,7 +1653,7 @@
         <v>14.17</v>
       </c>
     </row>
-    <row r="153" spans="1:2">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A153" s="3">
         <v>36022</v>
       </c>
@@ -1651,7 +1661,7 @@
         <v>13.47</v>
       </c>
     </row>
-    <row r="154" spans="1:2">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A154" s="3">
         <v>36053</v>
       </c>
@@ -1659,7 +1669,7 @@
         <v>15.03</v>
       </c>
     </row>
-    <row r="155" spans="1:2">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A155" s="3">
         <v>36083</v>
       </c>
@@ -1667,7 +1677,7 @@
         <v>14.46</v>
       </c>
     </row>
-    <row r="156" spans="1:2">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A156" s="3">
         <v>36114</v>
       </c>
@@ -1675,7 +1685,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="157" spans="1:2">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A157" s="3">
         <v>36144</v>
       </c>
@@ -1683,7 +1693,7 @@
         <v>11.35</v>
       </c>
     </row>
-    <row r="158" spans="1:2">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A158" s="3">
         <v>36175</v>
       </c>
@@ -1691,7 +1701,7 @@
         <v>12.52</v>
       </c>
     </row>
-    <row r="159" spans="1:2">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A159" s="3">
         <v>36206</v>
       </c>
@@ -1699,7 +1709,7 @@
         <v>12.01</v>
       </c>
     </row>
-    <row r="160" spans="1:2">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A160" s="3">
         <v>36234</v>
       </c>
@@ -1707,7 +1717,7 @@
         <v>14.68</v>
       </c>
     </row>
-    <row r="161" spans="1:2">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A161" s="3">
         <v>36265</v>
       </c>
@@ -1715,7 +1725,7 @@
         <v>17.309999999999999</v>
       </c>
     </row>
-    <row r="162" spans="1:2">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A162" s="3">
         <v>36295</v>
       </c>
@@ -1723,7 +1733,7 @@
         <v>17.72</v>
       </c>
     </row>
-    <row r="163" spans="1:2">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A163" s="3">
         <v>36326</v>
       </c>
@@ -1731,7 +1741,7 @@
         <v>17.920000000000002</v>
       </c>
     </row>
-    <row r="164" spans="1:2">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A164" s="3">
         <v>36356</v>
       </c>
@@ -1739,7 +1749,7 @@
         <v>20.100000000000001</v>
       </c>
     </row>
-    <row r="165" spans="1:2">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A165" s="3">
         <v>36387</v>
       </c>
@@ -1747,7 +1757,7 @@
         <v>21.28</v>
       </c>
     </row>
-    <row r="166" spans="1:2">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A166" s="3">
         <v>36418</v>
       </c>
@@ -1755,7 +1765,7 @@
         <v>23.8</v>
       </c>
     </row>
-    <row r="167" spans="1:2">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A167" s="3">
         <v>36448</v>
       </c>
@@ -1763,7 +1773,7 @@
         <v>22.69</v>
       </c>
     </row>
-    <row r="168" spans="1:2">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A168" s="3">
         <v>36479</v>
       </c>
@@ -1771,7 +1781,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="169" spans="1:2">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A169" s="3">
         <v>36509</v>
       </c>
@@ -1779,7 +1789,7 @@
         <v>26.1</v>
       </c>
     </row>
-    <row r="170" spans="1:2">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A170" s="3">
         <v>36540</v>
       </c>
@@ -1787,7 +1797,7 @@
         <v>27.26</v>
       </c>
     </row>
-    <row r="171" spans="1:2">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A171" s="3">
         <v>36571</v>
       </c>
@@ -1795,7 +1805,7 @@
         <v>29.37</v>
       </c>
     </row>
-    <row r="172" spans="1:2">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A172" s="3">
         <v>36600</v>
       </c>
@@ -1803,7 +1813,7 @@
         <v>29.84</v>
       </c>
     </row>
-    <row r="173" spans="1:2">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A173" s="3">
         <v>36631</v>
       </c>
@@ -1811,7 +1821,7 @@
         <v>25.72</v>
       </c>
     </row>
-    <row r="174" spans="1:2">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A174" s="3">
         <v>36661</v>
       </c>
@@ -1819,7 +1829,7 @@
         <v>28.79</v>
       </c>
     </row>
-    <row r="175" spans="1:2">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A175" s="3">
         <v>36692</v>
       </c>
@@ -1827,7 +1837,7 @@
         <v>31.82</v>
       </c>
     </row>
-    <row r="176" spans="1:2">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A176" s="3">
         <v>36722</v>
       </c>
@@ -1835,7 +1845,7 @@
         <v>29.7</v>
       </c>
     </row>
-    <row r="177" spans="1:2">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A177" s="3">
         <v>36753</v>
       </c>
@@ -1843,7 +1853,7 @@
         <v>31.26</v>
       </c>
     </row>
-    <row r="178" spans="1:2">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A178" s="3">
         <v>36784</v>
       </c>
@@ -1851,7 +1861,7 @@
         <v>33.880000000000003</v>
       </c>
     </row>
-    <row r="179" spans="1:2">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A179" s="3">
         <v>36814</v>
       </c>
@@ -1859,7 +1869,7 @@
         <v>33.11</v>
       </c>
     </row>
-    <row r="180" spans="1:2">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A180" s="3">
         <v>36845</v>
       </c>
@@ -1867,7 +1877,7 @@
         <v>34.42</v>
       </c>
     </row>
-    <row r="181" spans="1:2">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A181" s="3">
         <v>36875</v>
       </c>
@@ -1875,7 +1885,7 @@
         <v>28.44</v>
       </c>
     </row>
-    <row r="182" spans="1:2">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A182" s="3">
         <v>36906</v>
       </c>
@@ -1883,7 +1893,7 @@
         <v>29.59</v>
       </c>
     </row>
-    <row r="183" spans="1:2">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A183" s="3">
         <v>36937</v>
       </c>
@@ -1891,7 +1901,7 @@
         <v>29.61</v>
       </c>
     </row>
-    <row r="184" spans="1:2">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A184" s="3">
         <v>36965</v>
       </c>
@@ -1899,7 +1909,7 @@
         <v>27.25</v>
       </c>
     </row>
-    <row r="185" spans="1:2">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A185" s="3">
         <v>36996</v>
       </c>
@@ -1907,7 +1917,7 @@
         <v>27.49</v>
       </c>
     </row>
-    <row r="186" spans="1:2">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A186" s="3">
         <v>37026</v>
       </c>
@@ -1915,7 +1925,7 @@
         <v>28.63</v>
       </c>
     </row>
-    <row r="187" spans="1:2">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A187" s="3">
         <v>37057</v>
       </c>
@@ -1923,7 +1933,7 @@
         <v>27.6</v>
       </c>
     </row>
-    <row r="188" spans="1:2">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A188" s="3">
         <v>37087</v>
       </c>
@@ -1931,7 +1941,7 @@
         <v>26.43</v>
       </c>
     </row>
-    <row r="189" spans="1:2">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A189" s="3">
         <v>37118</v>
       </c>
@@ -1939,7 +1949,7 @@
         <v>27.37</v>
       </c>
     </row>
-    <row r="190" spans="1:2">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A190" s="3">
         <v>37149</v>
       </c>
@@ -1947,7 +1957,7 @@
         <v>26.2</v>
       </c>
     </row>
-    <row r="191" spans="1:2">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A191" s="3">
         <v>37179</v>
       </c>
@@ -1955,7 +1965,7 @@
         <v>22.17</v>
       </c>
     </row>
-    <row r="192" spans="1:2">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A192" s="3">
         <v>37210</v>
       </c>
@@ -1963,7 +1973,7 @@
         <v>19.64</v>
       </c>
     </row>
-    <row r="193" spans="1:2">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A193" s="3">
         <v>37240</v>
       </c>
@@ -1971,7 +1981,7 @@
         <v>19.39</v>
       </c>
     </row>
-    <row r="194" spans="1:2">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A194" s="3">
         <v>37271</v>
       </c>
@@ -1979,7 +1989,7 @@
         <v>19.72</v>
       </c>
     </row>
-    <row r="195" spans="1:2">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A195" s="3">
         <v>37302</v>
       </c>
@@ -1987,7 +1997,7 @@
         <v>20.72</v>
       </c>
     </row>
-    <row r="196" spans="1:2">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A196" s="3">
         <v>37330</v>
       </c>
@@ -1995,7 +2005,7 @@
         <v>24.53</v>
       </c>
     </row>
-    <row r="197" spans="1:2">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A197" s="3">
         <v>37361</v>
       </c>
@@ -2003,7 +2013,7 @@
         <v>26.18</v>
       </c>
     </row>
-    <row r="198" spans="1:2">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A198" s="3">
         <v>37391</v>
       </c>
@@ -2011,7 +2021,7 @@
         <v>27.04</v>
       </c>
     </row>
-    <row r="199" spans="1:2">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A199" s="3">
         <v>37422</v>
       </c>
@@ -2019,7 +2029,7 @@
         <v>25.52</v>
       </c>
     </row>
-    <row r="200" spans="1:2">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A200" s="3">
         <v>37452</v>
       </c>
@@ -2027,7 +2037,7 @@
         <v>26.97</v>
       </c>
     </row>
-    <row r="201" spans="1:2">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A201" s="3">
         <v>37483</v>
       </c>
@@ -2035,7 +2045,7 @@
         <v>28.39</v>
       </c>
     </row>
-    <row r="202" spans="1:2">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A202" s="3">
         <v>37514</v>
       </c>
@@ -2043,7 +2053,7 @@
         <v>29.66</v>
       </c>
     </row>
-    <row r="203" spans="1:2">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A203" s="3">
         <v>37544</v>
       </c>
@@ -2051,7 +2061,7 @@
         <v>28.84</v>
       </c>
     </row>
-    <row r="204" spans="1:2">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A204" s="3">
         <v>37575</v>
       </c>
@@ -2059,7 +2069,7 @@
         <v>26.35</v>
       </c>
     </row>
-    <row r="205" spans="1:2">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A205" s="3">
         <v>37605</v>
       </c>
@@ -2067,7 +2077,7 @@
         <v>29.46</v>
       </c>
     </row>
-    <row r="206" spans="1:2">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A206" s="3">
         <v>37636</v>
       </c>
@@ -2075,7 +2085,7 @@
         <v>32.950000000000003</v>
       </c>
     </row>
-    <row r="207" spans="1:2">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A207" s="3">
         <v>37667</v>
       </c>
@@ -2083,7 +2093,7 @@
         <v>35.83</v>
       </c>
     </row>
-    <row r="208" spans="1:2">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A208" s="3">
         <v>37695</v>
       </c>
@@ -2091,7 +2101,7 @@
         <v>33.51</v>
       </c>
     </row>
-    <row r="209" spans="1:2">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A209" s="3">
         <v>37726</v>
       </c>
@@ -2099,7 +2109,7 @@
         <v>28.17</v>
       </c>
     </row>
-    <row r="210" spans="1:2">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A210" s="3">
         <v>37756</v>
       </c>
@@ -2107,7 +2117,7 @@
         <v>28.11</v>
       </c>
     </row>
-    <row r="211" spans="1:2">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A211" s="3">
         <v>37787</v>
       </c>
@@ -2115,7 +2125,7 @@
         <v>30.66</v>
       </c>
     </row>
-    <row r="212" spans="1:2">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A212" s="3">
         <v>37817</v>
       </c>
@@ -2123,7 +2133,7 @@
         <v>30.76</v>
       </c>
     </row>
-    <row r="213" spans="1:2">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A213" s="3">
         <v>37848</v>
       </c>
@@ -2131,7 +2141,7 @@
         <v>31.57</v>
       </c>
     </row>
-    <row r="214" spans="1:2">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A214" s="3">
         <v>37879</v>
       </c>
@@ -2139,7 +2149,7 @@
         <v>28.31</v>
       </c>
     </row>
-    <row r="215" spans="1:2">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A215" s="3">
         <v>37909</v>
       </c>
@@ -2147,7 +2157,7 @@
         <v>30.34</v>
       </c>
     </row>
-    <row r="216" spans="1:2">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A216" s="3">
         <v>37940</v>
       </c>
@@ -2155,7 +2165,7 @@
         <v>31.11</v>
       </c>
     </row>
-    <row r="217" spans="1:2">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A217" s="3">
         <v>37970</v>
       </c>
@@ -2163,7 +2173,7 @@
         <v>32.130000000000003</v>
       </c>
     </row>
-    <row r="218" spans="1:2">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A218" s="3">
         <v>38001</v>
       </c>
@@ -2171,7 +2181,7 @@
         <v>34.31</v>
       </c>
     </row>
-    <row r="219" spans="1:2">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A219" s="3">
         <v>38032</v>
       </c>
@@ -2179,7 +2189,7 @@
         <v>34.69</v>
       </c>
     </row>
-    <row r="220" spans="1:2">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A220" s="3">
         <v>38061</v>
       </c>
@@ -2187,7 +2197,7 @@
         <v>36.74</v>
       </c>
     </row>
-    <row r="221" spans="1:2">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A221" s="3">
         <v>38092</v>
       </c>
@@ -2195,7 +2205,7 @@
         <v>36.75</v>
       </c>
     </row>
-    <row r="222" spans="1:2">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A222" s="3">
         <v>38122</v>
       </c>
@@ -2203,7 +2213,7 @@
         <v>40.28</v>
       </c>
     </row>
-    <row r="223" spans="1:2">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A223" s="3">
         <v>38153</v>
       </c>
@@ -2211,7 +2221,7 @@
         <v>38.03</v>
       </c>
     </row>
-    <row r="224" spans="1:2">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A224" s="3">
         <v>38183</v>
       </c>
@@ -2219,7 +2229,7 @@
         <v>40.78</v>
       </c>
     </row>
-    <row r="225" spans="1:2">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A225" s="3">
         <v>38214</v>
       </c>
@@ -2227,7 +2237,7 @@
         <v>44.9</v>
       </c>
     </row>
-    <row r="226" spans="1:2">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A226" s="3">
         <v>38245</v>
       </c>
@@ -2235,7 +2245,7 @@
         <v>45.94</v>
       </c>
     </row>
-    <row r="227" spans="1:2">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A227" s="3">
         <v>38275</v>
       </c>
@@ -2243,7 +2253,7 @@
         <v>53.28</v>
       </c>
     </row>
-    <row r="228" spans="1:2">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A228" s="3">
         <v>38306</v>
       </c>
@@ -2251,7 +2261,7 @@
         <v>48.47</v>
       </c>
     </row>
-    <row r="229" spans="1:2">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A229" s="3">
         <v>38336</v>
       </c>
@@ -2259,7 +2269,7 @@
         <v>43.15</v>
       </c>
     </row>
-    <row r="230" spans="1:2">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A230" s="3">
         <v>38367</v>
       </c>
@@ -2267,7 +2277,7 @@
         <v>46.84</v>
       </c>
     </row>
-    <row r="231" spans="1:2">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A231" s="3">
         <v>38398</v>
       </c>
@@ -2275,7 +2285,7 @@
         <v>48.15</v>
       </c>
     </row>
-    <row r="232" spans="1:2">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A232" s="3">
         <v>38426</v>
       </c>
@@ -2283,7 +2293,7 @@
         <v>54.19</v>
       </c>
     </row>
-    <row r="233" spans="1:2">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A233" s="3">
         <v>38457</v>
       </c>
@@ -2291,7 +2301,7 @@
         <v>52.98</v>
       </c>
     </row>
-    <row r="234" spans="1:2">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A234" s="3">
         <v>38487</v>
       </c>
@@ -2299,7 +2309,7 @@
         <v>49.83</v>
       </c>
     </row>
-    <row r="235" spans="1:2">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A235" s="3">
         <v>38518</v>
       </c>
@@ -2307,7 +2317,7 @@
         <v>56.35</v>
       </c>
     </row>
-    <row r="236" spans="1:2">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A236" s="3">
         <v>38548</v>
       </c>
@@ -2315,7 +2325,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="237" spans="1:2">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A237" s="3">
         <v>38579</v>
       </c>
@@ -2323,7 +2333,7 @@
         <v>64.989999999999995</v>
       </c>
     </row>
-    <row r="238" spans="1:2">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A238" s="3">
         <v>38610</v>
       </c>
@@ -2331,7 +2341,7 @@
         <v>65.59</v>
       </c>
     </row>
-    <row r="239" spans="1:2">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A239" s="3">
         <v>38640</v>
       </c>
@@ -2339,7 +2349,7 @@
         <v>62.26</v>
       </c>
     </row>
-    <row r="240" spans="1:2">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A240" s="3">
         <v>38671</v>
       </c>
@@ -2347,7 +2357,7 @@
         <v>58.32</v>
       </c>
     </row>
-    <row r="241" spans="1:2">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A241" s="3">
         <v>38701</v>
       </c>
@@ -2355,7 +2365,7 @@
         <v>59.41</v>
       </c>
     </row>
-    <row r="242" spans="1:2">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A242" s="3">
         <v>38732</v>
       </c>
@@ -2363,7 +2373,7 @@
         <v>65.489999999999995</v>
       </c>
     </row>
-    <row r="243" spans="1:2">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A243" s="3">
         <v>38763</v>
       </c>
@@ -2371,7 +2381,7 @@
         <v>61.63</v>
       </c>
     </row>
-    <row r="244" spans="1:2">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A244" s="3">
         <v>38791</v>
       </c>
@@ -2379,7 +2389,7 @@
         <v>62.69</v>
       </c>
     </row>
-    <row r="245" spans="1:2">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A245" s="3">
         <v>38822</v>
       </c>
@@ -2387,7 +2397,7 @@
         <v>69.44</v>
       </c>
     </row>
-    <row r="246" spans="1:2">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A246" s="3">
         <v>38852</v>
       </c>
@@ -2395,7 +2405,7 @@
         <v>70.84</v>
       </c>
     </row>
-    <row r="247" spans="1:2">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A247" s="3">
         <v>38883</v>
       </c>
@@ -2403,7 +2413,7 @@
         <v>70.95</v>
       </c>
     </row>
-    <row r="248" spans="1:2">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A248" s="3">
         <v>38913</v>
       </c>
@@ -2411,7 +2421,7 @@
         <v>74.41</v>
       </c>
     </row>
-    <row r="249" spans="1:2">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A249" s="3">
         <v>38944</v>
       </c>
@@ -2419,7 +2429,7 @@
         <v>73.040000000000006</v>
       </c>
     </row>
-    <row r="250" spans="1:2">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A250" s="3">
         <v>38975</v>
       </c>
@@ -2427,7 +2437,7 @@
         <v>63.8</v>
       </c>
     </row>
-    <row r="251" spans="1:2">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A251" s="3">
         <v>39005</v>
       </c>
@@ -2435,7 +2445,7 @@
         <v>58.89</v>
       </c>
     </row>
-    <row r="252" spans="1:2">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A252" s="3">
         <v>39036</v>
       </c>
@@ -2443,7 +2453,7 @@
         <v>59.08</v>
       </c>
     </row>
-    <row r="253" spans="1:2">
+    <row r="253" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A253" s="3">
         <v>39066</v>
       </c>
@@ -2451,7 +2461,7 @@
         <v>61.96</v>
       </c>
     </row>
-    <row r="254" spans="1:2">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A254" s="3">
         <v>39097</v>
       </c>
@@ -2459,7 +2469,7 @@
         <v>54.51</v>
       </c>
     </row>
-    <row r="255" spans="1:2">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A255" s="3">
         <v>39128</v>
       </c>
@@ -2467,7 +2477,7 @@
         <v>59.28</v>
       </c>
     </row>
-    <row r="256" spans="1:2">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A256" s="3">
         <v>39156</v>
       </c>
@@ -2475,7 +2485,7 @@
         <v>60.44</v>
       </c>
     </row>
-    <row r="257" spans="1:2">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A257" s="3">
         <v>39187</v>
       </c>
@@ -2483,7 +2493,7 @@
         <v>63.98</v>
       </c>
     </row>
-    <row r="258" spans="1:2">
+    <row r="258" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A258" s="3">
         <v>39217</v>
       </c>
@@ -2491,7 +2501,7 @@
         <v>63.46</v>
       </c>
     </row>
-    <row r="259" spans="1:2">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A259" s="3">
         <v>39248</v>
       </c>
@@ -2499,7 +2509,7 @@
         <v>67.489999999999995</v>
       </c>
     </row>
-    <row r="260" spans="1:2">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A260" s="3">
         <v>39278</v>
       </c>
@@ -2507,7 +2517,7 @@
         <v>74.12</v>
       </c>
     </row>
-    <row r="261" spans="1:2">
+    <row r="261" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A261" s="3">
         <v>39309</v>
       </c>
@@ -2515,7 +2525,7 @@
         <v>72.36</v>
       </c>
     </row>
-    <row r="262" spans="1:2">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A262" s="3">
         <v>39340</v>
       </c>
@@ -2523,7 +2533,7 @@
         <v>79.92</v>
       </c>
     </row>
-    <row r="263" spans="1:2">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A263" s="3">
         <v>39370</v>
       </c>
@@ -2531,7 +2541,7 @@
         <v>85.8</v>
       </c>
     </row>
-    <row r="264" spans="1:2">
+    <row r="264" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A264" s="3">
         <v>39401</v>
       </c>
@@ -2539,7 +2549,7 @@
         <v>94.77</v>
       </c>
     </row>
-    <row r="265" spans="1:2">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A265" s="3">
         <v>39431</v>
       </c>
@@ -2547,7 +2557,7 @@
         <v>91.69</v>
       </c>
     </row>
-    <row r="266" spans="1:2">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A266" s="3">
         <v>39462</v>
       </c>
@@ -2555,7 +2565,7 @@
         <v>92.97</v>
       </c>
     </row>
-    <row r="267" spans="1:2">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A267" s="3">
         <v>39493</v>
       </c>
@@ -2563,7 +2573,7 @@
         <v>95.39</v>
       </c>
     </row>
-    <row r="268" spans="1:2">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A268" s="3">
         <v>39522</v>
       </c>
@@ -2571,7 +2581,7 @@
         <v>105.45</v>
       </c>
     </row>
-    <row r="269" spans="1:2">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A269" s="3">
         <v>39553</v>
       </c>
@@ -2579,7 +2589,7 @@
         <v>112.58</v>
       </c>
     </row>
-    <row r="270" spans="1:2">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A270" s="3">
         <v>39583</v>
       </c>
@@ -2587,7 +2597,7 @@
         <v>125.4</v>
       </c>
     </row>
-    <row r="271" spans="1:2">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A271" s="3">
         <v>39614</v>
       </c>
@@ -2595,7 +2605,7 @@
         <v>133.88</v>
       </c>
     </row>
-    <row r="272" spans="1:2">
+    <row r="272" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A272" s="3">
         <v>39644</v>
       </c>
@@ -2603,7 +2613,7 @@
         <v>133.37</v>
       </c>
     </row>
-    <row r="273" spans="1:2">
+    <row r="273" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A273" s="3">
         <v>39675</v>
       </c>
@@ -2611,7 +2621,7 @@
         <v>116.67</v>
       </c>
     </row>
-    <row r="274" spans="1:2">
+    <row r="274" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A274" s="3">
         <v>39706</v>
       </c>
@@ -2619,7 +2629,7 @@
         <v>104.11</v>
       </c>
     </row>
-    <row r="275" spans="1:2">
+    <row r="275" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A275" s="3">
         <v>39736</v>
       </c>
@@ -2627,7 +2637,7 @@
         <v>76.61</v>
       </c>
     </row>
-    <row r="276" spans="1:2">
+    <row r="276" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A276" s="3">
         <v>39767</v>
       </c>
@@ -2635,7 +2645,7 @@
         <v>57.31</v>
       </c>
     </row>
-    <row r="277" spans="1:2">
+    <row r="277" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A277" s="3">
         <v>39797</v>
       </c>
@@ -2643,7 +2653,7 @@
         <v>41.12</v>
       </c>
     </row>
-    <row r="278" spans="1:2">
+    <row r="278" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A278" s="3">
         <v>39828</v>
       </c>
@@ -2651,7 +2661,7 @@
         <v>41.71</v>
       </c>
     </row>
-    <row r="279" spans="1:2">
+    <row r="279" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A279" s="3">
         <v>39859</v>
       </c>
@@ -2659,7 +2669,7 @@
         <v>39.090000000000003</v>
       </c>
     </row>
-    <row r="280" spans="1:2">
+    <row r="280" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A280" s="3">
         <v>39887</v>
       </c>
@@ -2667,7 +2677,7 @@
         <v>47.94</v>
       </c>
     </row>
-    <row r="281" spans="1:2">
+    <row r="281" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A281" s="3">
         <v>39918</v>
       </c>
@@ -2675,7 +2685,7 @@
         <v>49.65</v>
       </c>
     </row>
-    <row r="282" spans="1:2">
+    <row r="282" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A282" s="3">
         <v>39948</v>
       </c>
@@ -2683,7 +2693,7 @@
         <v>59.03</v>
       </c>
     </row>
-    <row r="283" spans="1:2">
+    <row r="283" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A283" s="3">
         <v>39979</v>
       </c>
@@ -2691,7 +2701,7 @@
         <v>69.64</v>
       </c>
     </row>
-    <row r="284" spans="1:2">
+    <row r="284" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A284" s="3">
         <v>40009</v>
       </c>
@@ -2699,7 +2709,7 @@
         <v>64.150000000000006</v>
       </c>
     </row>
-    <row r="285" spans="1:2">
+    <row r="285" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A285" s="3">
         <v>40040</v>
       </c>
@@ -2707,7 +2717,7 @@
         <v>71.05</v>
       </c>
     </row>
-    <row r="286" spans="1:2">
+    <row r="286" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A286" s="3">
         <v>40071</v>
       </c>
@@ -2715,7 +2725,7 @@
         <v>69.41</v>
       </c>
     </row>
-    <row r="287" spans="1:2">
+    <row r="287" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A287" s="3">
         <v>40101</v>
       </c>
@@ -2723,7 +2733,7 @@
         <v>75.72</v>
       </c>
     </row>
-    <row r="288" spans="1:2">
+    <row r="288" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A288" s="3">
         <v>40132</v>
       </c>
@@ -2731,7 +2741,7 @@
         <v>77.989999999999995</v>
       </c>
     </row>
-    <row r="289" spans="1:2">
+    <row r="289" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A289" s="3">
         <v>40162</v>
       </c>
@@ -2739,7 +2749,7 @@
         <v>74.47</v>
       </c>
     </row>
-    <row r="290" spans="1:2">
+    <row r="290" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A290" s="3">
         <v>40193</v>
       </c>
@@ -2747,7 +2757,7 @@
         <v>78.33</v>
       </c>
     </row>
-    <row r="291" spans="1:2">
+    <row r="291" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A291" s="3">
         <v>40224</v>
       </c>
@@ -2755,7 +2765,7 @@
         <v>76.39</v>
       </c>
     </row>
-    <row r="292" spans="1:2">
+    <row r="292" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A292" s="3">
         <v>40252</v>
       </c>
@@ -2763,7 +2773,7 @@
         <v>81.2</v>
       </c>
     </row>
-    <row r="293" spans="1:2">
+    <row r="293" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A293" s="3">
         <v>40283</v>
       </c>
@@ -2771,7 +2781,7 @@
         <v>84.29</v>
       </c>
     </row>
-    <row r="294" spans="1:2">
+    <row r="294" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A294" s="3">
         <v>40313</v>
       </c>
@@ -2779,7 +2789,7 @@
         <v>73.739999999999995</v>
       </c>
     </row>
-    <row r="295" spans="1:2">
+    <row r="295" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A295" s="3">
         <v>40344</v>
       </c>
@@ -2787,7 +2797,7 @@
         <v>75.34</v>
       </c>
     </row>
-    <row r="296" spans="1:2">
+    <row r="296" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A296" s="3">
         <v>40374</v>
       </c>
@@ -2795,7 +2805,7 @@
         <v>76.319999999999993</v>
       </c>
     </row>
-    <row r="297" spans="1:2">
+    <row r="297" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A297" s="3">
         <v>40405</v>
       </c>
@@ -2803,7 +2813,7 @@
         <v>76.599999999999994</v>
       </c>
     </row>
-    <row r="298" spans="1:2">
+    <row r="298" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A298" s="3">
         <v>40436</v>
       </c>
@@ -2811,7 +2821,7 @@
         <v>75.239999999999995</v>
       </c>
     </row>
-    <row r="299" spans="1:2">
+    <row r="299" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A299" s="3">
         <v>40466</v>
       </c>
@@ -2819,7 +2829,7 @@
         <v>81.89</v>
       </c>
     </row>
-    <row r="300" spans="1:2">
+    <row r="300" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A300" s="3">
         <v>40497</v>
       </c>
@@ -2827,7 +2837,7 @@
         <v>84.25</v>
       </c>
     </row>
-    <row r="301" spans="1:2">
+    <row r="301" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A301" s="3">
         <v>40527</v>
       </c>
@@ -2835,7 +2845,7 @@
         <v>89.15</v>
       </c>
     </row>
-    <row r="302" spans="1:2">
+    <row r="302" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A302" s="3">
         <v>40558</v>
       </c>
@@ -2843,7 +2853,7 @@
         <v>89.17</v>
       </c>
     </row>
-    <row r="303" spans="1:2">
+    <row r="303" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A303" s="3">
         <v>40589</v>
       </c>
@@ -2851,7 +2861,7 @@
         <v>88.58</v>
       </c>
     </row>
-    <row r="304" spans="1:2">
+    <row r="304" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A304" s="3">
         <v>40617</v>
       </c>
@@ -2859,7 +2869,7 @@
         <v>102.86</v>
       </c>
     </row>
-    <row r="305" spans="1:2">
+    <row r="305" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A305" s="3">
         <v>40648</v>
       </c>
@@ -2867,7 +2877,7 @@
         <v>109.53</v>
       </c>
     </row>
-    <row r="306" spans="1:2">
+    <row r="306" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A306" s="3">
         <v>40678</v>
       </c>
@@ -2875,7 +2885,7 @@
         <v>100.9</v>
       </c>
     </row>
-    <row r="307" spans="1:2">
+    <row r="307" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A307" s="3">
         <v>40709</v>
       </c>
@@ -2883,7 +2893,7 @@
         <v>96.26</v>
       </c>
     </row>
-    <row r="308" spans="1:2">
+    <row r="308" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A308" s="3">
         <v>40739</v>
       </c>
@@ -2891,7 +2901,7 @@
         <v>97.3</v>
       </c>
     </row>
-    <row r="309" spans="1:2">
+    <row r="309" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A309" s="3">
         <v>40770</v>
       </c>
@@ -2899,7 +2909,7 @@
         <v>86.33</v>
       </c>
     </row>
-    <row r="310" spans="1:2">
+    <row r="310" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A310" s="3">
         <v>40801</v>
       </c>
@@ -2907,7 +2917,7 @@
         <v>85.52</v>
       </c>
     </row>
-    <row r="311" spans="1:2">
+    <row r="311" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A311" s="3">
         <v>40831</v>
       </c>
@@ -2915,7 +2925,7 @@
         <v>86.32</v>
       </c>
     </row>
-    <row r="312" spans="1:2">
+    <row r="312" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A312" s="3">
         <v>40862</v>
       </c>
@@ -2923,7 +2933,7 @@
         <v>97.16</v>
       </c>
     </row>
-    <row r="313" spans="1:2">
+    <row r="313" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A313" s="3">
         <v>40892</v>
       </c>
@@ -2931,7 +2941,7 @@
         <v>98.56</v>
       </c>
     </row>
-    <row r="314" spans="1:2">
+    <row r="314" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A314" s="3">
         <v>40923</v>
       </c>
@@ -2939,7 +2949,7 @@
         <v>100.27</v>
       </c>
     </row>
-    <row r="315" spans="1:2">
+    <row r="315" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A315" s="3">
         <v>40954</v>
       </c>
@@ -2947,7 +2957,7 @@
         <v>102.2</v>
       </c>
     </row>
-    <row r="316" spans="1:2">
+    <row r="316" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A316" s="3">
         <v>40983</v>
       </c>
@@ -2955,7 +2965,7 @@
         <v>106.16</v>
       </c>
     </row>
-    <row r="317" spans="1:2">
+    <row r="317" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A317" s="3">
         <v>41014</v>
       </c>
@@ -2963,7 +2973,7 @@
         <v>103.32</v>
       </c>
     </row>
-    <row r="318" spans="1:2">
+    <row r="318" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A318" s="3">
         <v>41044</v>
       </c>
@@ -2971,7 +2981,7 @@
         <v>94.66</v>
       </c>
     </row>
-    <row r="319" spans="1:2">
+    <row r="319" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A319" s="3">
         <v>41075</v>
       </c>
@@ -2979,7 +2989,7 @@
         <v>82.3</v>
       </c>
     </row>
-    <row r="320" spans="1:2">
+    <row r="320" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A320" s="3">
         <v>41105</v>
       </c>
@@ -2987,7 +2997,7 @@
         <v>87.9</v>
       </c>
     </row>
-    <row r="321" spans="1:2">
+    <row r="321" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A321" s="3">
         <v>41136</v>
       </c>
@@ -2995,7 +3005,7 @@
         <v>94.13</v>
       </c>
     </row>
-    <row r="322" spans="1:2">
+    <row r="322" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A322" s="3">
         <v>41167</v>
       </c>
@@ -3003,7 +3013,7 @@
         <v>94.51</v>
       </c>
     </row>
-    <row r="323" spans="1:2">
+    <row r="323" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A323" s="3">
         <v>41197</v>
       </c>
@@ -3011,7 +3021,7 @@
         <v>89.49</v>
       </c>
     </row>
-    <row r="324" spans="1:2">
+    <row r="324" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A324" s="3">
         <v>41228</v>
       </c>
@@ -3019,7 +3029,7 @@
         <v>86.53</v>
       </c>
     </row>
-    <row r="325" spans="1:2">
+    <row r="325" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A325" s="3">
         <v>41258</v>
       </c>
@@ -3027,7 +3037,7 @@
         <v>87.86</v>
       </c>
     </row>
-    <row r="326" spans="1:2">
+    <row r="326" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A326" s="3">
         <v>41289</v>
       </c>
@@ -3035,7 +3045,7 @@
         <v>94.76</v>
       </c>
     </row>
-    <row r="327" spans="1:2">
+    <row r="327" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A327" s="3">
         <v>41320</v>
       </c>
@@ -3043,7 +3053,7 @@
         <v>95.31</v>
       </c>
     </row>
-    <row r="328" spans="1:2">
+    <row r="328" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A328" s="3">
         <v>41348</v>
       </c>
@@ -3051,7 +3061,7 @@
         <v>92.94</v>
       </c>
     </row>
-    <row r="329" spans="1:2">
+    <row r="329" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A329" s="3">
         <v>41379</v>
       </c>
@@ -3059,7 +3069,7 @@
         <v>92.02</v>
       </c>
     </row>
-    <row r="330" spans="1:2">
+    <row r="330" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A330" s="3">
         <v>41409</v>
       </c>
@@ -3067,7 +3077,7 @@
         <v>94.51</v>
       </c>
     </row>
-    <row r="331" spans="1:2">
+    <row r="331" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A331" s="3">
         <v>41440</v>
       </c>
@@ -3075,7 +3085,7 @@
         <v>95.77</v>
       </c>
     </row>
-    <row r="332" spans="1:2">
+    <row r="332" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A332" s="3">
         <v>41470</v>
       </c>
@@ -3083,7 +3093,7 @@
         <v>104.67</v>
       </c>
     </row>
-    <row r="333" spans="1:2">
+    <row r="333" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A333" s="3">
         <v>41501</v>
       </c>
@@ -3091,7 +3101,7 @@
         <v>106.57</v>
       </c>
     </row>
-    <row r="334" spans="1:2">
+    <row r="334" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A334" s="3">
         <v>41532</v>
       </c>
@@ -3099,7 +3109,7 @@
         <v>106.29</v>
       </c>
     </row>
-    <row r="335" spans="1:2">
+    <row r="335" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A335" s="3">
         <v>41562</v>
       </c>
@@ -3107,7 +3117,7 @@
         <v>100.54</v>
       </c>
     </row>
-    <row r="336" spans="1:2">
+    <row r="336" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A336" s="3">
         <v>41593</v>
       </c>
@@ -3115,7 +3125,7 @@
         <v>93.86</v>
       </c>
     </row>
-    <row r="337" spans="1:2">
+    <row r="337" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A337" s="3">
         <v>41623</v>
       </c>
@@ -3123,7 +3133,7 @@
         <v>97.63</v>
       </c>
     </row>
-    <row r="338" spans="1:2">
+    <row r="338" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A338" s="3">
         <v>41654</v>
       </c>
@@ -3131,7 +3141,7 @@
         <v>94.62</v>
       </c>
     </row>
-    <row r="339" spans="1:2">
+    <row r="339" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A339" s="3">
         <v>41685</v>
       </c>
@@ -3139,7 +3149,7 @@
         <v>100.82</v>
       </c>
     </row>
-    <row r="340" spans="1:2">
+    <row r="340" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A340" s="3">
         <v>41713</v>
       </c>
@@ -3147,7 +3157,7 @@
         <v>100.8</v>
       </c>
     </row>
-    <row r="341" spans="1:2">
+    <row r="341" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A341" s="3">
         <v>41744</v>
       </c>
@@ -3155,7 +3165,7 @@
         <v>102.07</v>
       </c>
     </row>
-    <row r="342" spans="1:2">
+    <row r="342" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A342" s="3">
         <v>41774</v>
       </c>
@@ -3163,7 +3173,7 @@
         <v>102.18</v>
       </c>
     </row>
-    <row r="343" spans="1:2">
+    <row r="343" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A343" s="3">
         <v>41805</v>
       </c>
@@ -3171,7 +3181,7 @@
         <v>105.79</v>
       </c>
     </row>
-    <row r="344" spans="1:2">
+    <row r="344" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A344" s="3">
         <v>41835</v>
       </c>
@@ -3179,7 +3189,7 @@
         <v>103.59</v>
       </c>
     </row>
-    <row r="345" spans="1:2">
+    <row r="345" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A345" s="3">
         <v>41866</v>
       </c>
@@ -3187,7 +3197,7 @@
         <v>96.54</v>
       </c>
     </row>
-    <row r="346" spans="1:2">
+    <row r="346" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A346" s="3">
         <v>41897</v>
       </c>
@@ -3195,7 +3205,7 @@
         <v>93.21</v>
       </c>
     </row>
-    <row r="347" spans="1:2">
+    <row r="347" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A347" s="3">
         <v>41927</v>
       </c>
@@ -3203,7 +3213,7 @@
         <v>84.4</v>
       </c>
     </row>
-    <row r="348" spans="1:2">
+    <row r="348" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A348" s="3">
         <v>41958</v>
       </c>
@@ -3211,7 +3221,7 @@
         <v>75.790000000000006</v>
       </c>
     </row>
-    <row r="349" spans="1:2">
+    <row r="349" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A349" s="3">
         <v>41988</v>
       </c>
@@ -3219,7 +3229,7 @@
         <v>59.29</v>
       </c>
     </row>
-    <row r="350" spans="1:2">
+    <row r="350" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A350" s="3">
         <v>42019</v>
       </c>
@@ -3227,7 +3237,7 @@
         <v>47.22</v>
       </c>
     </row>
-    <row r="351" spans="1:2">
+    <row r="351" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A351" s="3">
         <v>42050</v>
       </c>
@@ -3235,21 +3245,80 @@
         <v>50.58</v>
       </c>
     </row>
-    <row r="352" spans="1:2">
+    <row r="352" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A352" s="3">
         <v>42078</v>
       </c>
       <c r="B352">
         <v>47.82</v>
+      </c>
+    </row>
+    <row r="353" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A353" s="3">
+        <v>42109</v>
+      </c>
+      <c r="B353">
+        <v>54.45</v>
+      </c>
+    </row>
+    <row r="354" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A354" s="3">
+        <v>42139</v>
+      </c>
+      <c r="B354">
+        <v>59.27</v>
+      </c>
+    </row>
+    <row r="355" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A355" s="3">
+        <v>42170</v>
+      </c>
+      <c r="B355">
+        <v>59.82</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A356" s="3">
+        <v>42200</v>
+      </c>
+      <c r="B356">
+        <v>50.9</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A357" s="3">
+        <v>42231</v>
+      </c>
+      <c r="B357">
+        <v>42.87</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A358" s="3">
+        <v>42262</v>
+      </c>
+      <c r="B358">
+        <v>45.48</v>
+      </c>
+    </row>
+    <row r="359" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A359" s="3">
+        <v>42292</v>
+      </c>
+      <c r="B359">
+        <v>46.22</v>
+      </c>
+    </row>
+    <row r="360" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A360" s="3">
+        <v>42323</v>
+      </c>
+      <c r="B360">
+        <v>42.39</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>